<commit_message>
update mapping terms analysis
</commit_message>
<xml_diff>
--- a/src/ontology/mappings/OBO-space/07.03.2025-mapped-terms-analysis.xlsx
+++ b/src/ontology/mappings/OBO-space/07.03.2025-mapped-terms-analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\fathoni\github\molsim-ontology\src\ontology\mappings\OBO-space\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DE30D0-873C-4BE1-97CF-AFA4C7C30548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE1489A-92D2-43F6-95DB-33F53DFBAFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="-18120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,6 +90,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{9BE479D2-25A7-47E9-9BA9-755436D2733A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fathoni Musyaffa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+discard/map/import</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="H57" authorId="0" shapeId="0" xr:uid="{EEE3CCF8-CAA3-4D5F-A8C6-5B20EB50EEE5}">
       <text>
         <r>
@@ -110,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="592">
   <si>
     <t>subject_label</t>
   </si>
@@ -2918,9 +2942,6 @@
 </t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>P-value as result of one of the processing steps described. Specify in the description, which processing step it was.</t>
   </si>
   <si>
@@ -3101,9 +3122,6 @@
     <t>Changes in version imply substantive changes in content rather than differences in format. This property is intended to be used with non-literal values. This property is an inverse property of Is Version Of. A related resource that is a version, edition, or adaptation of the described resource.</t>
   </si>
   <si>
-    <t>likely not</t>
-  </si>
-  <si>
     <t>A channel formed as a result of a stream cutting through a meander neck.</t>
   </si>
   <si>
@@ -3132,6 +3150,99 @@
   </si>
   <si>
     <t>(not resolvable)</t>
+  </si>
+  <si>
+    <t>similar to IAO:0000010</t>
+  </si>
+  <si>
+    <t>similar to FIX:0000327</t>
+  </si>
+  <si>
+    <t>similar to SBO:0000393</t>
+  </si>
+  <si>
+    <t>similar to IDO:0000607</t>
+  </si>
+  <si>
+    <t>similar to NCIT:C54165</t>
+  </si>
+  <si>
+    <t>similar to SBO:0000212</t>
+  </si>
+  <si>
+    <t>similar to FBcv:0003108</t>
+  </si>
+  <si>
+    <t>similar to MS:1000531</t>
+  </si>
+  <si>
+    <t>similar to OMIT:0003464</t>
+  </si>
+  <si>
+    <t>relevant/anything similar?</t>
+  </si>
+  <si>
+    <t>similar to APOLLO:SV_00000422</t>
+  </si>
+  <si>
+    <t xml:space="preserve">similar to NCIT:C28901 </t>
+  </si>
+  <si>
+    <t>similar to ExO:0000090</t>
+  </si>
+  <si>
+    <t>most likely no</t>
+  </si>
+  <si>
+    <t>similar to SIO:000510</t>
+  </si>
+  <si>
+    <t>possibly, but the ontology does not seems to be maintained/mature enough</t>
+  </si>
+  <si>
+    <t>discard (as there are other terms containing the term model?)</t>
+  </si>
+  <si>
+    <t>similar to NCIT:C16866</t>
+  </si>
+  <si>
+    <t>similar to MI:0077</t>
+  </si>
+  <si>
+    <t>similar to NCIT:C16921</t>
+  </si>
+  <si>
+    <t>similar to CHEBI:32588</t>
+  </si>
+  <si>
+    <t>similar to NCIT:C47679</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Principal Component Analysis </t>
+  </si>
+  <si>
+    <t>similar to OMIT:0021132</t>
+  </si>
+  <si>
+    <t>similar to NCIT:C49291</t>
+  </si>
+  <si>
+    <t>similar to MS:1002072, NCIT:C44185</t>
+  </si>
+  <si>
+    <t>similar to MS:1002072,OBI:0000175</t>
+  </si>
+  <si>
+    <t>similar to OBI:0000175, NCIT:C44185</t>
+  </si>
+  <si>
+    <t>all of these seems similar: PATO:0001025, CVDO:0000193</t>
+  </si>
+  <si>
+    <t>all of these seems similar: SWO:0004000, SLSO:0001174, DCTERMS:hasVersion, OIO:hasVersion</t>
+  </si>
+  <si>
+    <t>all of these seem similar: ENVO:00000523, NCIT:C47877, STATO:0000633</t>
   </si>
 </sst>
 </file>
@@ -3375,7 +3486,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3458,7 +3569,7 @@
         <v>16</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>17</v>
@@ -3488,7 +3599,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -3504,8 +3615,8 @@
       <c r="E3" s="7" t="s">
         <v>481</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>552</v>
+      <c r="F3" s="6" t="s">
+        <v>589</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>27</v>
@@ -3535,7 +3646,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
@@ -3549,7 +3660,10 @@
         <v>32</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>551</v>
+        <v>550</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>590</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>33</v>
@@ -3579,7 +3693,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
@@ -3593,10 +3707,10 @@
         <v>38</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>553</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>591</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>39</v>
@@ -3626,7 +3740,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>42</v>
       </c>
@@ -3640,8 +3754,9 @@
         <v>44</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>554</v>
-      </c>
+        <v>552</v>
+      </c>
+      <c r="F6" s="6"/>
       <c r="H6" s="3" t="s">
         <v>45</v>
       </c>
@@ -3667,7 +3782,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>47</v>
       </c>
@@ -3681,8 +3796,9 @@
         <v>50</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>555</v>
-      </c>
+        <v>553</v>
+      </c>
+      <c r="F7" s="6"/>
       <c r="H7" s="3" t="s">
         <v>51</v>
       </c>
@@ -3711,7 +3827,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -3725,7 +3841,10 @@
         <v>55</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>556</v>
+        <v>554</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>591</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>56</v>
@@ -3755,7 +3874,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>59</v>
       </c>
@@ -3769,8 +3888,9 @@
         <v>62</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>557</v>
-      </c>
+        <v>555</v>
+      </c>
+      <c r="F9" s="6"/>
       <c r="H9" s="3" t="s">
         <v>63</v>
       </c>
@@ -3799,7 +3919,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -3815,6 +3935,9 @@
       <c r="E10" s="7" t="s">
         <v>481</v>
       </c>
+      <c r="F10" s="6" t="s">
+        <v>590</v>
+      </c>
       <c r="H10" s="3" t="s">
         <v>67</v>
       </c>
@@ -3843,7 +3966,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -3857,8 +3980,9 @@
         <v>68</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>558</v>
-      </c>
+        <v>556</v>
+      </c>
+      <c r="F11" s="6"/>
       <c r="H11" s="3" t="s">
         <v>69</v>
       </c>
@@ -3887,7 +4011,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -3901,7 +4025,10 @@
         <v>72</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>559</v>
+        <v>557</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>590</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>73</v>
@@ -3931,7 +4058,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>76</v>
       </c>
@@ -3945,8 +4072,9 @@
         <v>78</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>560</v>
-      </c>
+        <v>558</v>
+      </c>
+      <c r="F13" s="6"/>
       <c r="H13" s="3" t="s">
         <v>79</v>
       </c>
@@ -3975,7 +4103,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -3989,7 +4117,10 @@
         <v>82</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>561</v>
+        <v>559</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>591</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>83</v>
@@ -4019,7 +4150,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
@@ -4033,7 +4164,10 @@
         <v>84</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>562</v>
+        <v>560</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>590</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>85</v>
@@ -4099,18 +4233,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="J100" sqref="J100"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.81640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.6328125" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.90625" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.6328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6328125" style="7" customWidth="1"/>
-    <col min="6" max="7" width="16.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="72.36328125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="16.6328125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" style="1" customWidth="1"/>
     <col min="8" max="8" width="114.1796875" style="1" customWidth="1"/>
     <col min="9" max="9" width="48.6328125" style="1" customWidth="1"/>
     <col min="10" max="10" width="33.7265625" style="1" customWidth="1"/>
@@ -4123,7 +4258,7 @@
     <col min="17" max="17" width="23.7265625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4139,8 +4274,8 @@
       <c r="E1" s="6" t="s">
         <v>472</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>475</v>
+      <c r="F1" s="6" t="s">
+        <v>570</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>466</v>
@@ -4176,7 +4311,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>90</v>
       </c>
@@ -4223,7 +4358,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>97</v>
       </c>
@@ -4237,10 +4372,10 @@
         <v>100</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>546</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>547</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>548</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>101</v>
@@ -4270,7 +4405,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>104</v>
       </c>
@@ -4317,7 +4452,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>111</v>
       </c>
@@ -4364,7 +4499,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>118</v>
       </c>
@@ -4380,6 +4515,9 @@
       <c r="E6" s="10" t="s">
         <v>473</v>
       </c>
+      <c r="F6" s="6" t="s">
+        <v>581</v>
+      </c>
       <c r="H6" s="3" t="s">
         <v>121</v>
       </c>
@@ -4411,7 +4549,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>123</v>
       </c>
@@ -4427,6 +4565,9 @@
       <c r="E7" s="7" t="s">
         <v>474</v>
       </c>
+      <c r="F7" s="6" t="s">
+        <v>582</v>
+      </c>
       <c r="H7" s="3" t="s">
         <v>126</v>
       </c>
@@ -4458,7 +4599,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>128</v>
       </c>
@@ -4505,7 +4646,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>128</v>
       </c>
@@ -4519,7 +4660,7 @@
         <v>135</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>469</v>
@@ -4558,7 +4699,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>140</v>
       </c>
@@ -4575,10 +4716,10 @@
         <v>478</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>469</v>
+        <v>576</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>467</v>
+        <v>577</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>143</v>
@@ -4611,7 +4752,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>147</v>
       </c>
@@ -4658,7 +4799,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>152</v>
       </c>
@@ -4705,7 +4846,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>159</v>
       </c>
@@ -4752,7 +4893,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>166</v>
       </c>
@@ -4799,7 +4940,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>171</v>
       </c>
@@ -4846,7 +4987,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>176</v>
       </c>
@@ -4893,7 +5034,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>180</v>
       </c>
@@ -4909,6 +5050,9 @@
       <c r="E17" s="7" t="s">
         <v>484</v>
       </c>
+      <c r="F17" s="6" t="s">
+        <v>568</v>
+      </c>
       <c r="H17" s="3" t="s">
         <v>183</v>
       </c>
@@ -4937,7 +5081,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>186</v>
       </c>
@@ -4984,7 +5128,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>191</v>
       </c>
@@ -5031,7 +5175,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>198</v>
       </c>
@@ -5047,6 +5191,9 @@
       <c r="E20" s="7" t="s">
         <v>487</v>
       </c>
+      <c r="F20" s="6" t="s">
+        <v>563</v>
+      </c>
       <c r="H20" s="3" t="s">
         <v>201</v>
       </c>
@@ -5078,7 +5225,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>205</v>
       </c>
@@ -5092,7 +5239,7 @@
         <v>207</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>208</v>
@@ -5122,7 +5269,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>211</v>
       </c>
@@ -5136,7 +5283,10 @@
         <v>213</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>544</v>
+        <v>543</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>580</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>214</v>
@@ -5166,7 +5316,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>159</v>
       </c>
@@ -5210,7 +5360,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>221</v>
       </c>
@@ -5254,7 +5404,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>180</v>
       </c>
@@ -5270,8 +5420,8 @@
       <c r="E25" s="7" t="s">
         <v>490</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>491</v>
+      <c r="F25" s="6" t="s">
+        <v>561</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>227</v>
@@ -5304,7 +5454,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>229</v>
       </c>
@@ -5318,10 +5468,13 @@
         <v>231</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>492</v>
+        <v>491</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>588</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>232</v>
@@ -5351,7 +5504,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>198</v>
       </c>
@@ -5365,10 +5518,10 @@
         <v>234</v>
       </c>
       <c r="E27" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>493</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>494</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>235</v>
@@ -5401,7 +5554,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>166</v>
       </c>
@@ -5415,7 +5568,10 @@
         <v>238</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>495</v>
+        <v>494</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>562</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>239</v>
@@ -5448,7 +5604,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>140</v>
       </c>
@@ -5462,7 +5618,10 @@
         <v>242</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>496</v>
+        <v>495</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>575</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>243</v>
@@ -5495,7 +5654,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>211</v>
       </c>
@@ -5509,10 +5668,13 @@
         <v>248</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>498</v>
+        <v>497</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>579</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>249</v>
@@ -5542,7 +5704,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>250</v>
       </c>
@@ -5556,7 +5718,7 @@
         <v>253</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>254</v>
@@ -5589,7 +5751,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>159</v>
       </c>
@@ -5603,7 +5765,7 @@
         <v>257</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>258</v>
@@ -5636,7 +5798,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>260</v>
       </c>
@@ -5650,7 +5812,7 @@
         <v>263</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>264</v>
@@ -5683,7 +5845,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>266</v>
       </c>
@@ -5697,7 +5859,7 @@
         <v>269</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>270</v>
@@ -5730,7 +5892,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>152</v>
       </c>
@@ -5744,7 +5906,10 @@
         <v>273</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>503</v>
+        <v>502</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>567</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>274</v>
@@ -5777,7 +5942,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>276</v>
       </c>
@@ -5791,7 +5956,7 @@
         <v>279</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>280</v>
@@ -5824,7 +5989,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>90</v>
       </c>
@@ -5838,7 +6003,7 @@
         <v>283</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>284</v>
@@ -5871,7 +6036,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>286</v>
       </c>
@@ -5885,7 +6050,10 @@
         <v>289</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>506</v>
+        <v>505</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>569</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>290</v>
@@ -5918,7 +6086,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>292</v>
       </c>
@@ -5932,7 +6100,7 @@
         <v>295</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>296</v>
@@ -5965,7 +6133,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>140</v>
       </c>
@@ -5979,7 +6147,10 @@
         <v>298</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>508</v>
+        <v>507</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>574</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>299</v>
@@ -6012,7 +6183,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>229</v>
       </c>
@@ -6026,7 +6197,10 @@
         <v>302</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>509</v>
+        <v>508</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>587</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>303</v>
@@ -6059,7 +6233,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>123</v>
       </c>
@@ -6073,7 +6247,10 @@
         <v>306</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>510</v>
+        <v>509</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>581</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>307</v>
@@ -6106,7 +6283,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>309</v>
       </c>
@@ -6120,7 +6297,7 @@
         <v>312</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="H43" s="3" t="s">
         <v>313</v>
@@ -6153,7 +6330,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>317</v>
       </c>
@@ -6167,7 +6344,7 @@
         <v>320</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>321</v>
@@ -6200,7 +6377,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>323</v>
       </c>
@@ -6208,13 +6385,16 @@
         <v>324</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>325</v>
+        <v>583</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>326</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>513</v>
+        <v>512</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>584</v>
       </c>
       <c r="H45" s="3" t="s">
         <v>327</v>
@@ -6247,7 +6427,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>329</v>
       </c>
@@ -6261,7 +6441,7 @@
         <v>332</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>333</v>
@@ -6294,7 +6474,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>335</v>
       </c>
@@ -6308,7 +6488,10 @@
         <v>338</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>515</v>
+        <v>514</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>566</v>
       </c>
       <c r="H47" s="3" t="s">
         <v>339</v>
@@ -6341,7 +6524,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>341</v>
       </c>
@@ -6355,7 +6538,7 @@
         <v>344</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>469</v>
@@ -6394,7 +6577,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>347</v>
       </c>
@@ -6408,7 +6591,7 @@
         <v>350</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>351</v>
@@ -6441,7 +6624,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>147</v>
       </c>
@@ -6455,7 +6638,10 @@
         <v>354</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>518</v>
+        <v>517</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>573</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>355</v>
@@ -6488,7 +6674,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>357</v>
       </c>
@@ -6502,7 +6688,7 @@
         <v>360</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>361</v>
@@ -6535,7 +6721,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>363</v>
       </c>
@@ -6549,7 +6735,7 @@
         <v>366</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>367</v>
@@ -6582,7 +6768,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>90</v>
       </c>
@@ -6596,7 +6782,7 @@
         <v>369</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>469</v>
@@ -6635,7 +6821,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>372</v>
       </c>
@@ -6649,10 +6835,10 @@
         <v>375</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>376</v>
@@ -6682,7 +6868,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>229</v>
       </c>
@@ -6696,7 +6882,10 @@
         <v>377</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>524</v>
+        <v>523</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>586</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>378</v>
@@ -6729,7 +6918,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>382</v>
       </c>
@@ -6743,7 +6932,7 @@
         <v>384</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>385</v>
@@ -6776,7 +6965,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>140</v>
       </c>
@@ -6790,12 +6979,12 @@
         <v>389</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>541</v>
-      </c>
-      <c r="F57" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="F57" s="6" t="s">
         <v>469</v>
       </c>
-      <c r="G57" s="1" t="s">
+      <c r="G57" s="6" t="s">
         <v>467</v>
       </c>
       <c r="H57" s="3" t="s">
@@ -6829,7 +7018,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>286</v>
       </c>
@@ -6845,6 +7034,9 @@
       <c r="E58" s="7" t="s">
         <v>481</v>
       </c>
+      <c r="F58" s="6" t="s">
+        <v>572</v>
+      </c>
       <c r="H58" s="3" t="s">
         <v>393</v>
       </c>
@@ -6876,7 +7068,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>397</v>
       </c>
@@ -6923,7 +7115,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>97</v>
       </c>
@@ -6939,6 +7131,9 @@
       <c r="E60" s="7" t="s">
         <v>481</v>
       </c>
+      <c r="F60" s="6" t="s">
+        <v>571</v>
+      </c>
       <c r="H60" s="3" t="s">
         <v>405</v>
       </c>
@@ -6970,7 +7165,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>407</v>
       </c>
@@ -6993,7 +7188,7 @@
         <v>467</v>
       </c>
       <c r="H61" s="8" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I61" s="1" t="s">
         <v>411</v>
@@ -7023,7 +7218,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>323</v>
       </c>
@@ -7039,6 +7234,9 @@
       <c r="E62" s="7" t="s">
         <v>481</v>
       </c>
+      <c r="F62" s="6" t="s">
+        <v>585</v>
+      </c>
       <c r="H62" s="3" t="s">
         <v>413</v>
       </c>
@@ -7070,7 +7268,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>415</v>
       </c>
@@ -7084,10 +7282,10 @@
         <v>417</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I63" s="1" t="s">
         <v>418</v>
@@ -7117,7 +7315,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>335</v>
       </c>
@@ -7131,10 +7329,13 @@
         <v>419</v>
       </c>
       <c r="E64" s="11" t="s">
-        <v>539</v>
+        <v>538</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>565</v>
       </c>
       <c r="H64" s="8" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I64" s="1" t="s">
         <v>420</v>
@@ -7161,7 +7362,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>198</v>
       </c>
@@ -7175,7 +7376,10 @@
         <v>422</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>564</v>
       </c>
       <c r="H65" s="3" t="s">
         <v>423</v>
@@ -7205,7 +7409,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>140</v>
       </c>
@@ -7219,10 +7423,13 @@
         <v>425</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>538</v>
+        <v>537</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>578</v>
       </c>
       <c r="H66" s="8" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>426</v>
@@ -7252,7 +7459,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>427</v>
       </c>
@@ -7266,7 +7473,7 @@
         <v>429</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="H67" s="3" t="s">
         <v>430</v>
@@ -7299,7 +7506,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>432</v>
       </c>
@@ -7313,7 +7520,7 @@
         <v>434</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="H68" s="3" t="s">
         <v>435</v>
@@ -7346,7 +7553,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>437</v>
       </c>
@@ -7360,7 +7567,7 @@
         <v>439</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H69" s="3" t="s">
         <v>440</v>
@@ -7393,7 +7600,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>229</v>
       </c>
@@ -7407,7 +7614,7 @@
         <v>442</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H70" s="3" t="s">
         <v>443</v>
@@ -7440,7 +7647,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>445</v>
       </c>
@@ -7454,10 +7661,10 @@
         <v>447</v>
       </c>
       <c r="E71" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="H71" s="8" t="s">
         <v>535</v>
-      </c>
-      <c r="H71" s="8" t="s">
-        <v>536</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>86</v>
@@ -7484,7 +7691,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>90</v>
       </c>
@@ -7498,7 +7705,13 @@
         <v>448</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>531</v>
+        <v>530</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="G72" s="6" t="s">
+        <v>467</v>
       </c>
       <c r="H72" s="5" t="s">
         <v>449</v>
@@ -7528,7 +7741,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:17" ht="13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>452</v>
       </c>
@@ -7542,7 +7755,7 @@
         <v>455</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>469</v>
@@ -7578,7 +7791,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:17" ht="13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>459</v>
       </c>
@@ -7592,7 +7805,7 @@
         <v>461</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>469</v>

</xml_diff>

<commit_message>
add missing terms from biosio, modify terms hierarchy
</commit_message>
<xml_diff>
--- a/src/ontology/mappings/OBO-space/07.03.2025-mapped-terms-analysis.xlsx
+++ b/src/ontology/mappings/OBO-space/07.03.2025-mapped-terms-analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\fathoni\github\molsim-ontology\src\ontology\mappings\OBO-space\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B16150A-A89B-4C78-B1DE-26C6A46BF82C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C5CAF8-4C2B-4829-B294-8A2A423C5F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3536,7 +3536,7 @@
   <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add no-intermediates extraction from iao/ncit/stato
</commit_message>
<xml_diff>
--- a/src/ontology/mappings/OBO-space/07.03.2025-mapped-terms-analysis.xlsx
+++ b/src/ontology/mappings/OBO-space/07.03.2025-mapped-terms-analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\fathoni\github\molsim-ontology\src\ontology\mappings\OBO-space\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C5CAF8-4C2B-4829-B294-8A2A423C5F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04933AA5-434C-4B81-80AB-AD2F1DB2912A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3536,7 +3536,7 @@
   <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4310,8 +4310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R74"/>
   <sheetViews>
-    <sheetView topLeftCell="C53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -5597,7 +5597,7 @@
       <c r="C27" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="13" t="s">
         <v>234</v>
       </c>
       <c r="E27" s="7" t="s">
@@ -6227,7 +6227,7 @@
       <c r="C40" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" s="13" t="s">
         <v>298</v>
       </c>
       <c r="E40" s="7" t="s">

</xml_diff>

<commit_message>
add definitions for application programs
</commit_message>
<xml_diff>
--- a/src/ontology/mappings/OBO-space/07.03.2025-mapped-terms-analysis.xlsx
+++ b/src/ontology/mappings/OBO-space/07.03.2025-mapped-terms-analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\fathoni\github\molsim-ontology\src\ontology\mappings\OBO-space\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04933AA5-434C-4B81-80AB-AD2F1DB2912A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6186F73C-7751-407A-9D98-08218A04C994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="-18120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Property" sheetId="1" r:id="rId1"/>
@@ -3269,9 +3269,6 @@
     <t>all of these seem similar: ENVO:00000523, NCIT:C47877, STATO:0000633</t>
   </si>
   <si>
-    <t>discard - possibly due to irrelevance, scope mismatch, maintenance/quality issues</t>
-  </si>
-  <si>
     <t>need to be discussed further</t>
   </si>
   <si>
@@ -3279,6 +3276,9 @@
   </si>
   <si>
     <t>hierarchy relevant?</t>
+  </si>
+  <si>
+    <t>discard - due to irrelevance, scope mismatch, maintenance/quality issues</t>
   </si>
 </sst>
 </file>
@@ -3535,8 +3535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3572,7 +3572,7 @@
         <v>472</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>475</v>
@@ -3944,7 +3944,7 @@
       <c r="C9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="12" t="s">
         <v>62</v>
       </c>
       <c r="E9" s="7" t="s">
@@ -4266,12 +4266,12 @@
     </row>
     <row r="19" spans="4:25" x14ac:dyDescent="0.25">
       <c r="D19" s="12" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
     </row>
     <row r="20" spans="4:25" x14ac:dyDescent="0.25">
       <c r="D20" s="13" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="25" spans="4:25" x14ac:dyDescent="0.25">
@@ -4311,7 +4311,7 @@
   <dimension ref="A1:R74"/>
   <sheetViews>
     <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C71" sqref="C71:D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -4352,7 +4352,7 @@
         <v>472</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>570</v>

</xml_diff>